<commit_message>
Cleaned up code outputs
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexbindas/Documents/BU/2023/CS777/termpaper/cs777-termpaper/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D5D765-E1A2-2443-89DC-0179747A7FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00136BA3-CE08-B04A-B9AF-3CC4D79C464B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27100" windowHeight="15100" xr2:uid="{F8C45C39-9EA8-9B43-9C0F-A758C27E4B77}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20640" windowHeight="15100" xr2:uid="{F8C45C39-9EA8-9B43-9C0F-A758C27E4B77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2303,7 +2303,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>